<commit_message>
Adding SFML, entries into gitignore, refactoring and more names in an excel file for future use.
</commit_message>
<xml_diff>
--- a/resources/scripts/names.xlsx
+++ b/resources/scripts/names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\preppers-worldsim\src\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\preppers-worldsim\resources\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="285">
   <si>
     <t>english</t>
   </si>
@@ -855,6 +855,30 @@
   </si>
   <si>
     <t>Adrianna</t>
+  </si>
+  <si>
+    <t>Adelard</t>
+  </si>
+  <si>
+    <t>Adolphe</t>
+  </si>
+  <si>
+    <t>Adrien</t>
+  </si>
+  <si>
+    <t>Agnes</t>
+  </si>
+  <si>
+    <t>Adeline</t>
+  </si>
+  <si>
+    <t>Antoine</t>
+  </si>
+  <si>
+    <t>Antoinette</t>
+  </si>
+  <si>
+    <t>Ariel</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,6 +1415,12 @@
       <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1438,6 +1468,12 @@
       <c r="O5" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1482,6 +1518,12 @@
       <c r="O6" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="P6" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1526,6 +1568,12 @@
       <c r="O7" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1570,6 +1618,9 @@
       <c r="O8" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1613,6 +1664,9 @@
       </c>
       <c r="O9" s="1" t="s">
         <v>72</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">

</xml_diff>